<commit_message>
add February agenda HTML file and update resident directory
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/03-march-hh/resident-directory/2025-03-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/03-march-hh/resident-directory/2025-03-heritage-resident-directory.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/03-march-hh/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="918" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F172BB20-8D02-46F6-A328-A0C974644950}"/>
+  <xr:revisionPtr revIDLastSave="923" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D1FB138-20DA-4787-80A7-F0AADF95FB6A}"/>
   <bookViews>
-    <workbookView xWindow="-18997" yWindow="-98" windowWidth="19095" windowHeight="12795" tabRatio="754" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="residents" sheetId="1" r:id="rId1"/>
-    <sheet name="directory" sheetId="6" r:id="rId2"/>
+    <sheet name="Residents" sheetId="1" r:id="rId1"/>
+    <sheet name="Directory" sheetId="6" r:id="rId2"/>
     <sheet name="birthdays" sheetId="12" r:id="rId3"/>
     <sheet name="Family" sheetId="16" r:id="rId4"/>
     <sheet name="No Family" sheetId="17" r:id="rId5"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="1110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="1110">
   <si>
     <t>First Name</t>
   </si>
@@ -8930,7 +8930,7 @@
       <c r="I1004" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:AA2 C7:D8 F7:H8 C9:H10 C11:E11 G11:H11 C12:H17 C18:AA51 D52:E53 C3:H6 I3:AA17 C54:AA75">
+  <conditionalFormatting sqref="C2:AA2 C3:H6 I3:AA17 C7:D8 F7:H8 C9:H10 C11:E11 G11:H11 C12:H17 C18:AA51 D52:E53 C54:AA75">
     <cfRule type="expression" dxfId="22" priority="1">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
@@ -9847,28 +9847,28 @@
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C12:E12 G12:AA12">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>"ISEVEN(ROW()"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C15:I15 K15:AB15 A27:J27">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
+      <formula>"ISEVEN(ROW()"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:AA2">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:AA11">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:AA24">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>"ISEVEN(ROW()"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:AA2">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>"ISEVEN(ROW()"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:E12 G12:AA12">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9886,7 +9886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C4F1CA-A107-47E1-B61D-684F7BB5060E}">
   <dimension ref="A1:Z173"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" showRuler="0" view="pageLayout" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
@@ -9919,23 +9919,23 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="str" cm="1">
-        <f t="array" ref="A2:A75">CONCATENATE(residents!A2:A75, " ", residents!B2:B75)</f>
+        <f t="array" ref="A2:A75">CONCATENATE(Residents!A2:A75, " ", Residents!B2:B75)</f>
         <v>Patrick Alexander</v>
       </c>
       <c r="B2" s="11" t="str" cm="1">
-        <f t="array" ref="B2:B75">residents!D2:D75</f>
+        <f t="array" ref="B2:B75">Residents!D2:D75</f>
         <v>230 C</v>
       </c>
       <c r="C2" s="11" t="str" cm="1">
-        <f t="array" ref="C2:C75">residents!E2:E75</f>
+        <f t="array" ref="C2:C75">Residents!E2:E75</f>
         <v>415 567-0419</v>
       </c>
       <c r="D2" s="11" t="str" cm="1">
-        <f t="array" ref="D2:D75">residents!F2:F75</f>
+        <f t="array" ref="D2:D75">Residents!F2:F75</f>
         <v>baimp@earthlink.net</v>
       </c>
       <c r="E2" s="12" t="str" cm="1">
-        <f t="array" ref="E2:E75">residents!I2:I75</f>
+        <f t="array" ref="E2:E75">Residents!I2:I75</f>
         <v>07/27</v>
       </c>
     </row>
@@ -12453,7 +12453,7 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="str" cm="1">
         <f t="array" ref="A1:B74">_xlfn.LET(
-    _xlpm.data, residents!A2:I75,
+    _xlpm.data, Residents!A2:I75,
     _xlpm.firstNames, INDEX(_xlpm.data, _xlfn.SEQUENCE(ROWS(_xlpm.data)), 1),
     _xlpm.lastNames, INDEX(_xlpm.data, _xlfn.SEQUENCE(ROWS(_xlpm.data)), 2),
     _xlpm.dates, INDEX(_xlpm.data, _xlfn.SEQUENCE(ROWS(_xlpm.data)), 9),
@@ -16165,11 +16165,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C4CAD2-851C-4D78-8B2D-D5100B32C514}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -16270,7 +16270,18 @@
         <v>1097</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C17" r:id="rId1" xr:uid="{33405957-C986-435E-B4F7-B48E571E3812}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update March resident directory and mailing documents: fix links and update contact information
</commit_message>
<xml_diff>
--- a/3-1-heritage/0-heritage-happenings/2025/03-march-hh/resident-directory/2025-03-heritage-resident-directory.xlsx
+++ b/3-1-heritage/0-heritage-happenings/2025/03-march-hh/resident-directory/2025-03-heritage-resident-directory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/03-march-hh/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="925" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D7263FC-3790-44C2-B448-E847F3A166DE}"/>
+  <xr:revisionPtr revIDLastSave="934" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8543DCB2-E37D-4995-87CA-0270EBB6AD6A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Residents" sheetId="1" r:id="rId1"/>
@@ -3324,9 +3324,6 @@
     <t>Sinclair</t>
   </si>
   <si>
-    <t>patricksinclair@yahoo.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Karen </t>
   </si>
   <si>
@@ -3381,13 +3378,16 @@
     <t>415 235-1375</t>
   </si>
   <si>
-    <t>jmnaughton1946@gmail.com</t>
-  </si>
-  <si>
     <t>02/12</t>
   </si>
   <si>
     <t>236 M</t>
+  </si>
+  <si>
+    <t>jimnaughton1946@gmail.com</t>
+  </si>
+  <si>
+    <t>patrickstclair@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -3775,35 +3775,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEAEA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEAEA"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <b/>
@@ -4021,6 +3993,20 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFD9D9D9"/>
           <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEAEA"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4264,8 +4250,8 @@
   <dimension ref="A1:I1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75:XFD75"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5010,7 +4996,7 @@
         <v>19</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>163</v>
@@ -5330,7 +5316,7 @@
         <v>19</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>231</v>
@@ -5561,22 +5547,22 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B52" s="17" t="s">
         <v>1096</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="D52" s="1" t="s">
         <v>1097</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>1098</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="F52" s="39" t="s">
         <v>1099</v>
       </c>
-      <c r="F52" s="39" t="s">
+      <c r="I52" s="53" t="s">
         <v>1100</v>
-      </c>
-      <c r="I52" s="53" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5584,19 +5570,19 @@
         <v>848</v>
       </c>
       <c r="B53" s="17" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>1097</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>1098</v>
-      </c>
       <c r="E53" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F53" s="40" t="s">
+        <v>1104</v>
+      </c>
+      <c r="I53" s="53" t="s">
         <v>1102</v>
-      </c>
-      <c r="F53" s="40" t="s">
-        <v>1103</v>
-      </c>
-      <c r="I53" s="53" t="s">
-        <v>1104</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
@@ -8917,7 +8903,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:AA2 C3:H6 I3:AA17 C7:D8 F7:H8 C9:H10 C11:E11 G11:H11 C12:H17 C18:AA51 D52:E53 C54:AA75">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8928,7 +8914,7 @@
     <hyperlink ref="F13" r:id="rId4" xr:uid="{592A1B3B-B2F7-4CDC-BDAC-D1AD979F0536}"/>
     <hyperlink ref="F55" r:id="rId5" xr:uid="{EA80CD83-9791-49E5-9CC4-F2AA9892E575}"/>
     <hyperlink ref="F21" r:id="rId6" xr:uid="{DFF8D86C-B09F-4E2D-97B8-F45B63E33AAA}"/>
-    <hyperlink ref="F53" r:id="rId7" xr:uid="{A7FBD182-2FD6-410C-9DE6-4164C35EF8C5}"/>
+    <hyperlink ref="F53" r:id="rId7" display="jmnaughton1946@gmail.com" xr:uid="{A7FBD182-2FD6-410C-9DE6-4164C35EF8C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId8"/>
@@ -9814,52 +9800,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A8:AB8">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:AC10 A13:AC13 K38:AC38 A39:J39">
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:AC18">
-    <cfRule type="expression" dxfId="11" priority="15">
+    <cfRule type="expression" dxfId="7" priority="15">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:AC23">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:E12 G12:AA12">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:I15 K15:AB15 A27:J27">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:AA2">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:AA11">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:AA24">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:AA30">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9872,8 +9858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C4F1CA-A107-47E1-B61D-684F7BB5060E}">
   <dimension ref="A1:Z173"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" showZeros="0" showRuler="0" view="pageLayout" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -10786,7 +10772,7 @@
         <v>415 235-1375</v>
       </c>
       <c r="D53" s="43" t="str">
-        <v>jmnaughton1946@gmail.com</v>
+        <v>jimnaughton1946@gmail.com</v>
       </c>
       <c r="E53" s="43" t="str">
         <v>02/12</v>
@@ -12404,12 +12390,12 @@
   </sheetData>
   <phoneticPr fontId="24" type="noConversion"/>
   <conditionalFormatting sqref="A2:E74">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13049,7 +13035,7 @@
   <sheetViews>
     <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -14235,52 +14221,52 @@
     <sortCondition ref="E2:E100"/>
   </sortState>
   <conditionalFormatting sqref="D17:D18">
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="22" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="21" priority="8">
+    <cfRule type="expression" dxfId="17" priority="8">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D33">
-    <cfRule type="expression" dxfId="20" priority="10">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="19" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="18" priority="7">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="17" priority="6">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62:D96">
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98:D100">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="14" priority="9">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14619,11 +14605,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAA4147-474C-47CD-A0DD-4C67000E8368}">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71:XFD71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -15341,7 +15327,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="11" t="s">
         <v>790</v>
       </c>
@@ -15352,7 +15338,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="11" t="s">
         <v>728</v>
       </c>
@@ -15363,7 +15349,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="11" t="s">
         <v>854</v>
       </c>
@@ -15374,7 +15360,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="11" t="s">
         <v>734</v>
       </c>
@@ -15385,7 +15371,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="11" t="s">
         <v>823</v>
       </c>
@@ -15396,7 +15382,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
         <v>1078</v>
       </c>
@@ -15407,40 +15393,40 @@
         <v>742</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="11" t="s">
         <v>1063</v>
       </c>
       <c r="B71" s="11" t="s">
         <v>1068</v>
       </c>
-      <c r="D71" s="11" t="s">
+      <c r="C71" s="11" t="s">
         <v>1067</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="11" t="s">
         <v>1069</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>1001</v>
       </c>
-      <c r="D72" s="11" t="s">
+      <c r="C72" s="11" t="s">
         <v>1070</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="11" t="s">
         <v>1064</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>1071</v>
       </c>
-      <c r="D73" s="11" t="s">
+      <c r="C73" s="11" t="s">
         <v>1072</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
         <v>1066</v>
       </c>
@@ -15468,8 +15454,8 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33:E36"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -15938,7 +15924,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -16154,8 +16140,8 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -16199,13 +16185,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>1088</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>1089</v>
-      </c>
       <c r="C3" s="11" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>1065</v>
@@ -16218,25 +16204,25 @@
       <c r="B4" s="11" t="s">
         <v>1083</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>1084</v>
+      <c r="C4" s="38" t="s">
+        <v>1105</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>658</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>161</v>
@@ -16247,13 +16233,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>1091</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>1092</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -16267,6 +16253,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C17" r:id="rId1" xr:uid="{33405957-C986-435E-B4F7-B48E571E3812}"/>
+    <hyperlink ref="C4" r:id="rId2" display="patrickstclaire@yahoo.com" xr:uid="{CC05467B-C936-4890-9DCC-181A092DC390}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>